<commit_message>
New RU localization version
</commit_message>
<xml_diff>
--- a/CustomLocalization/Localization/RogueTech/RU/ArtilleryUnits/LocalizationDef.xlsx
+++ b/CustomLocalization/Localization/RogueTech/RU/ArtilleryUnits/LocalizationDef.xlsx
@@ -44,11 +44,11 @@
   </si>
   <si>
     <t xml:space="preserve">The Archer 8L is a prototype chassis designed to provide fire support with 2 Arrow IV Launchers loaded with Incendiary Missiles and the newly developed Guardian ECM and Stealth Armor.
-&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 1.15.&lt;/color&gt;&lt;/b&gt;</t>
+&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 1.16.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">Archer 8L - прототип меха огневой поддержки, вооруженный двумя пусковыми установками Arrow IV с зажигательными боеприпасами и оснащенный недавно разработанной Guardian ECM и Stealth Armor.
-&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 1.15.&lt;/color&gt;&lt;/b&gt;</t>
+&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 1.16.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t>chassisdef_archer_ARC-8L.StockRole</t>
@@ -82,11 +82,11 @@
   </si>
   <si>
     <t xml:space="preserve">The C3 variant takes the 'Mech's long range fire support to a new level by removing both of the LRM-15 launchers and replacing them with an Arrow IV artillery system, allowing the Catapult to stay a safe distance from the battlefield.
-&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 1.12.&lt;/color&gt;&lt;/b&gt;</t>
+&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 1.13.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">Вариант C3 подымает огневую поддержку дальнего действия меха на новый уровень, удаляя обе пусковые установки LRM-15 и заменяя их артиллерийской системой Arrow IV, позволяя катапульте оставаться на безопасном расстоянии от поля битвы. 
-&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 1.12.&lt;/color&gt;&lt;/b&gt;</t>
+&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 1.13.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t>chassisdef_catapult_CPLT-C3.StockRole</t>
@@ -195,11 +195,11 @@
   </si>
   <si>
     <t xml:space="preserve">First unleashed by the Terran Hegemony in 2460, the Helepolis is a ponderous BattleMech designed to deliver artillery fire. The 'Mech was proven ineffective on multiple occasions and, following the destruction of the production facilities in 2775, the design was lost during the Succession Wars. The HEP-2H dates to 2488.
-&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 1.1.&lt;/color&gt;&lt;/b&gt;</t>
+&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 1.11.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">Впервые выпущенный Терранской Гегемонией в 2460 году, Helepolis является громоздким мехом, предназначенным для артиллерийского огня. Мех во многих случаях показывал свою неэффективность, а после разрушения производственных мощностей в 2775 году дизайн был утерян во время Войн за Наследие. HEP-2H датируется 2488 годом. 
-&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 1.1.&lt;/color&gt;&lt;/b&gt;</t>
+&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 1.11.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t>chassisdef_helepolis_HEP-2H.StockRole</t>
@@ -224,11 +224,11 @@
   </si>
   <si>
     <t xml:space="preserve">Built during the Amaris civil war, the Mackie 9Hb was a stopgap attempt to solve the SLDF's sudden dearth of advanced assault mechs. By taking Mackie 9H's from the remaining Hegemony stockpiles and upgrading them with surplus parts, the SLDF hoped to create a multi role assault mech for rear echelon and support duties; potentially freeing up better equipped machines that could be used on the frontlines. Equipped with 2 Thumper Artillery pieces and a cockpit command console, the 9Hb functions as both a command mech and an Artillery support platform. Though this design functions well as a support unit, it performs poorly in direct combat. Particularly devastating is the lack of CASE around the ammo magazines, a consequence of the rushed design process.
-&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 1.18.&lt;/color&gt;&lt;/b&gt;</t>
+&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 1.2.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">Построенный во время гражданской войны с Амарисом, Mackie 9Hb - это временная попытка решить внезапную нехватку SLDF передовых штурмовых мехов. Взяв Mackie 9H из оставшихся запасов Гегемонии и модернизировав его с помощью лишних запчастей, SLDF надеялся создать многоцелевой штурмовой мех для заднего эшелона и вспомогательных операций, потенциально освобождая лучше оборудованные машины для передовой. Оснащенный двумя Thumper Artillery и командирской консолью, -9Hb функционирует как командный мех и платформа артиллерийской поддержки. Хотя дизайн хорошо работает как вспомогательный юнит, он плохо работает в прямом бою. Особенно губительным является отсутствие CASE в секциях с боеприпасами, что является следствием спешного процесса проектирования. 
-&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 1.18.&lt;/color&gt;&lt;/b&gt;</t>
+&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 1.2.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t>chassisdef_mackie_MSK-9Hb.StockRole</t>
@@ -259,11 +259,11 @@
   </si>
   <si>
     <t xml:space="preserve">A clan buster refit developed with Comstar’s mothballed 9Hb’s, the 9Hc was an attempt to fix the failings of it’s predecessor design in a cheap and easy to maintain upgrade package. Identifying the lack of CASE and adequate secondary weapons as the key weaknesses, the Comguard designers disregarded the other weakness – the designs slow ground speed – as being of lesser importance. The designers selected an Endo Steel skeleton as the preferred option, rejecting other more expensive solutions. CASE was installed for both ammo magazines and the designers upgraded the medium lasers to ER versions; installing an extra 3 in the process with double heat sinks incorporated to balance out the heat spike. The 5 completed prototypes served with distinction on Tukayyid, though the design never reached production status; with only 2 other conversions finished before the Word of Blake seized Terra and the remaining stocks of 9Hb’s. .
-&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 1.2.&lt;/color&gt;&lt;/b&gt;</t>
+&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 1.22.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">Рефит замороженного проекта 9Hb от КомСтара. 9Нс - это попытка исправить ошибки своего предшественника, сделав дизайн дешевле и легче в эксплуатации. Определив нехватку CASE и наличие адекватного вспомогательного оружия ключевыми уязвимостями, инженеры КомГвардии пренебрегли другими - низкой скоростью - сочтя это менее значимым. Инженеры выбрали скелет из эндостали как основу, отказавшись от других более дорогих решений. CASE установлен в оба компонента с боеприпасами плюс инженеры усовершенствовали Medium Lasers до ER-версий, добавив к ним ещё 3 в процессе. Система Double Heatsinks компенсирует повышенный нагрев. 5 законченных прототипов прекрасно проявили себя на Токайдо, хотя вариант в серийное производство так и не пошел. И до того, как Слово Блейка захватило Терру и оставшиеся на ней модели -9Hb, только 2 меха успели переоборудовать в -9Hc. 
-&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 1.2.&lt;/color&gt;&lt;/b&gt;</t>
+&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 1.22.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t>chassisdef_mackie_MSK-9Hc.StockRole</t>
@@ -291,11 +291,11 @@
   </si>
   <si>
     <t xml:space="preserve">The Naga is a fire-support successor to the first-generation Woodsman OmniMech, but is an oddity in many ways. Most of what could be pod space for the design is actually taken up by a pair of fixed Arrow IV Artillery Systems. 
-&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 1.1.&lt;/color&gt;&lt;/b&gt;</t>
+&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 1.13.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">Naga является наследником первых поколений омнимехов Woodsman, мехов огневой поддержки, но имеет ряд отличий. Большая часть полезной нагрузки отведена под пару установок Arrow IV.
-&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 1.1.&lt;/color&gt;&lt;/b&gt;</t>
+&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 1.13.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t>chassisdef_naga_NGA-A.StockRole</t>
@@ -1373,11 +1373,11 @@
   </si>
   <si>
     <t xml:space="preserve">After his son was killed in the Taurian Concordat invasion of the Federated Suns, Benedict St. James had his VTR-9K refitted with experimental weapons and equipment to allow him to take his revenge. Replacing the standard weapons with a Long Tom Cannon and two Medium X-Pulse Lasers, St. James' Victor can inflict massive amounts of damage on his prey. The 'Mech's jump jets had to be removed to make way for the weapons load, and technicians equipped it with a patchwork of Ferro-Fibrous and Standard Armor as another weight saving measure. A Supercharger mounted on the engine provides the Victor with unexpected bursts of speed.
-&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 1.17.&lt;/color&gt;&lt;/b&gt;</t>
+&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 1.19.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">После того как его сына убили во время вторжения Федеративных Солнц в Таурианский Конкордат, Бенедикт Сент-Джеймс поклялся отомстить и для этого переоборудовал свой VTR-9K, снабдив того новыми экспериментальными технологиями. Заменив стандартное оружие на массивную пушку Long Tom и два средних X-Pulse лазера, мех Сент-Джеймса Victor способен обрушить огромную разрушительную мощь на головы своих врагов. Прыжковые двигатели пришлось удалить, чтобы освободить место для вооружения, плюс техи установили  ферроволокно и стандартную броню с той же целью. Supercharger установленный в двигатель Victor’а даёт тому буст скорости, которого никак не ожидаешь от подобного меха.
-&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 1.17.&lt;/color&gt;&lt;/b&gt;</t>
+&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 1.19.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t>chassisdef_victor_VTR-9K2.StockRole</t>
@@ -1465,11 +1465,11 @@
   </si>
   <si>
     <t xml:space="preserve">The earliest version used standard heat sinks and its Primitive Engine could only manage 30 km/h. This proved to be a challenge as the early Helepolis needed to completely stop to fire the Sniper artillery and then start moving again before counter-battery fire could destroy the unit. Twenty and a half tons of Primitive Armor protected the Helepolis from enemy fire. The weight and bulk of the primitive systems prevented the designers from installing the long range missiles used on later models.
-&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 0.88.&lt;/color&gt;&lt;/b&gt;</t>
+&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 0.89.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">На первую модель ставились одинарные теплопоглотители, а его примитивный двигатель разгонял меха только до 30 км/ч, что приводило к серьезным проблемам, так как ранние модели Helepolis не всегда успевали сменить позицию до того, пока их не накроют контрбатарейным огнем. Мех защищали 20.5 тонн примитивной брони, а вес и объем примитивных систем вооружения не позволили проектировщикам установить ракеты дальнего радиуса действия, как это было сделано на более поздних моделях. 
-&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 0.88.&lt;/color&gt;&lt;/b&gt;</t>
+&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 0.89.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t>chassisdef_helepolis_HEP-1H.StockRole</t>
@@ -1485,11 +1485,11 @@
   </si>
   <si>
     <t xml:space="preserve">The Helepolis is built around an Armstrong Industries Sniper Artillery Piece. The accurate, long-range fire makes it effective against static defenses. The 'Mech does carry some backup weapons to augment its screening forces. It can defend itself with a Coventry Starfire LRM-10 and Nova Large Laser. If an enemy gets close, the MechWarrior can call upon a Thunderstroke SRM-6 and a Starflash Medium Laser. This 2625 model upgrades the Large Laser to an ER Large Laser.
-&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 1.1.&lt;/color&gt;&lt;/b&gt;</t>
+&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 1.11.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">Helepolis собран вокруг артиллерийской установки Sniper производства Armstrong Industries. Точный дальний огонь делает его эффективным против защитных сооружений. Мех так же имеет вспомогательное вооружение, и может помочь своим силам прикрытия. В этом ему на дальних дистанциях ему помогает установка LRM-10 модели Coventry Starfire и большой лазер Nova. На ближней дистанции пилот может использовать средний лазер модели Starflash и SRM-6 Thunderstroke. У этой модели 2625 года большой лазер заменен на более дальнобойный. 
-&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 1.1.&lt;/color&gt;&lt;/b&gt;</t>
+&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 1.11.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t>chassisdef_helepolis_HEP-3H.StockRole</t>
@@ -1505,11 +1505,11 @@
   </si>
   <si>
     <t xml:space="preserve">This variant was introduced much more recently by Vining Engineering and Salvage Team. VEST rebuilt a factory on Solaris VII after the Word of Blake had left that world. There, they began to produce an upgraded version of the Helepolis. This upgrade of the 3H is built on an Endo Steel frame. It is powered by a 300-rated Light Fusion Engine that gives it a top speed of 64 km/h, though this necessitated splitting the missile launcher into two LRM-5s.
-&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 1.1.&lt;/color&gt;&lt;/b&gt;</t>
+&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 1.11.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">Этот вариант был представлен совсем недавно компанией Vining Engineering and Salvage Team (VEST). Когда Слово Блейка покинули Solaris VII, VEST восстановила разрушенный в этом мире завод. Там они начали выпускать улучшенную версию Helepolis. Взяв за основу модель -3H, новый -4H имеет каркас из эндостали. Питаемый двигателем Light Fusion Engine рейтинга 300, мех разгоняется до 64 км/ч, хотя чтобы достичь этого пришлось разделить ракетную пусковую установку на две LRM-5. 
-&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 1.1.&lt;/color&gt;&lt;/b&gt;</t>
+&lt;b&gt;&lt;color=#e62e00&gt;Drop Cost Multiplier: 1.11.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t>chassisdef_helepolis_HEP-4H.StockRole</t>
@@ -1574,11 +1574,14 @@
 Andrey Qorf
 Evgeniy Bidzhakov
 Ilhiz Zigangirov
+Boris Belior Burmyshev
+Podkhod engapproach Inzhenernyy
 Supporters:
 Evgeniy Invader Boyarinev
 Kirill Rorih Ivanov
 Vladimir Voha Peters
-Vyacheslav Battlemaster Zhandarov</t>
+Vyacheslav Battlemaster Zhandarov
+Sergey 0h0tnichek Kuznetsov</t>
   </si>
 </sst>
 </file>
@@ -1592,12 +1595,17 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1617,12 +1625,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="3" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
   </cellXfs>
@@ -1919,10 +1931,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D290"/>
+  <dimension ref="A1:F290"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A274" workbookViewId="0">
-      <selection activeCell="C285" sqref="C285"/>
+    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
+      <selection activeCell="C287" sqref="C287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1930,8 +1942,8 @@
     <col min="1" max="1" width="43" customWidth="1" style="2"/>
     <col min="2" max="2" width="82.42578125" customWidth="1" style="5"/>
     <col min="3" max="3" width="69" customWidth="1" style="5"/>
-    <col min="4" max="5" width="9.140625" customWidth="1" style="2"/>
-    <col min="6" max="16384" width="9.140625" customWidth="1" style="2"/>
+    <col min="4" max="6" width="9.140625" customWidth="1" style="2"/>
+    <col min="7" max="16384" width="9.140625" customWidth="1" style="2"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="1">
@@ -1976,19 +1988,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" s="4" customFormat="1">
-      <c r="A4" s="4" t="s">
+    <row r="4" s="7" customFormat="1">
+      <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="8"/>
     </row>
     <row r="5" s="3" customFormat="1">
       <c r="A5" s="3" t="s">
@@ -2046,19 +2059,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" s="4" customFormat="1">
-      <c r="A9" s="4" t="s">
+    <row r="9" s="7" customFormat="1">
+      <c r="A9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="8"/>
     </row>
     <row r="10" s="3" customFormat="1">
       <c r="A10" s="3" t="s">
@@ -2326,19 +2340,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" s="4" customFormat="1">
-      <c r="A29" s="4" t="s">
+    <row r="29" s="7" customFormat="1">
+      <c r="A29" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D29" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" s="8"/>
     </row>
     <row r="30" s="3" customFormat="1">
       <c r="A30" s="3" t="s">
@@ -2382,19 +2397,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" s="4" customFormat="1">
-      <c r="A33" s="4" t="s">
+    <row r="33" s="7" customFormat="1">
+      <c r="A33" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D33" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D33" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F33" s="8"/>
     </row>
     <row r="34" s="3" customFormat="1">
       <c r="A34" s="3" t="s">
@@ -2452,19 +2468,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" s="4" customFormat="1">
-      <c r="A38" s="4" t="s">
+    <row r="38" s="7" customFormat="1">
+      <c r="A38" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="D38" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D38" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F38" s="8"/>
     </row>
     <row r="39" s="3" customFormat="1">
       <c r="A39" s="3" t="s">
@@ -2522,19 +2539,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" s="4" customFormat="1">
-      <c r="A43" s="4" t="s">
+    <row r="43" s="7" customFormat="1">
+      <c r="A43" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D43" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D43" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F43" s="8"/>
     </row>
     <row r="44" s="3" customFormat="1">
       <c r="A44" s="3" t="s">
@@ -2592,19 +2610,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" s="4" customFormat="1">
-      <c r="A48" s="4" t="s">
+    <row r="48" s="7" customFormat="1">
+      <c r="A48" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B48" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C48" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D48" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D48" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F48" s="8"/>
     </row>
     <row r="49" s="3" customFormat="1">
       <c r="A49" s="3" t="s">
@@ -2662,19 +2681,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" s="4" customFormat="1">
-      <c r="A53" s="4" t="s">
+    <row r="53" s="7" customFormat="1">
+      <c r="A53" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="B53" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C53" s="6" t="s">
+      <c r="C53" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D53" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D53" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F53" s="8"/>
     </row>
     <row r="54" s="3" customFormat="1">
       <c r="A54" s="3" t="s">
@@ -2732,19 +2752,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" s="4" customFormat="1">
-      <c r="A58" s="4" t="s">
+    <row r="58" s="7" customFormat="1">
+      <c r="A58" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="B58" s="6" t="s">
+      <c r="B58" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="C58" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D58" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D58" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F58" s="8"/>
     </row>
     <row r="59" s="3" customFormat="1">
       <c r="A59" s="3" t="s">
@@ -2802,19 +2823,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" s="4" customFormat="1">
-      <c r="A63" s="4" t="s">
+    <row r="63" s="7" customFormat="1">
+      <c r="A63" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="B63" s="6" t="s">
+      <c r="B63" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="C63" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D63" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D63" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F63" s="8"/>
     </row>
     <row r="64" s="3" customFormat="1">
       <c r="A64" s="3" t="s">
@@ -3446,19 +3468,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="109" s="4" customFormat="1">
-      <c r="A109" s="4" t="s">
+    <row r="109" s="7" customFormat="1">
+      <c r="A109" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="B109" s="6" t="s">
+      <c r="B109" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C109" s="6" t="s">
+      <c r="C109" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D109" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D109" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F109" s="8"/>
     </row>
     <row r="110" s="3" customFormat="1">
       <c r="A110" s="3" t="s">
@@ -3488,19 +3511,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="112" s="4" customFormat="1">
-      <c r="A112" s="4" t="s">
+    <row r="112" s="7" customFormat="1">
+      <c r="A112" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="B112" s="6" t="s">
+      <c r="B112" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C112" s="6" t="s">
+      <c r="C112" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D112" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D112" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F112" s="8"/>
     </row>
     <row r="113" s="3" customFormat="1">
       <c r="A113" s="3" t="s">
@@ -3656,19 +3680,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="124" s="4" customFormat="1">
-      <c r="A124" s="4" t="s">
+    <row r="124" s="7" customFormat="1">
+      <c r="A124" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="B124" s="6" t="s">
+      <c r="B124" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C124" s="6" t="s">
+      <c r="C124" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D124" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D124" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F124" s="8"/>
     </row>
     <row r="125" s="3" customFormat="1">
       <c r="A125" s="3" t="s">
@@ -3698,19 +3723,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="127" s="4" customFormat="1">
-      <c r="A127" s="4" t="s">
+    <row r="127" s="7" customFormat="1">
+      <c r="A127" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="B127" s="6" t="s">
+      <c r="B127" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C127" s="6" t="s">
+      <c r="C127" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D127" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D127" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F127" s="8"/>
     </row>
     <row r="128" s="3" customFormat="1">
       <c r="A128" s="3" t="s">
@@ -3740,19 +3766,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="130" s="4" customFormat="1">
-      <c r="A130" s="4" t="s">
+    <row r="130" s="7" customFormat="1">
+      <c r="A130" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="B130" s="6" t="s">
+      <c r="B130" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C130" s="6" t="s">
+      <c r="C130" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="D130" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D130" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F130" s="8"/>
     </row>
     <row r="131" s="3" customFormat="1">
       <c r="A131" s="3" t="s">
@@ -3782,19 +3809,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="133" s="4" customFormat="1">
-      <c r="A133" s="4" t="s">
+    <row r="133" s="7" customFormat="1">
+      <c r="A133" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="B133" s="6" t="s">
+      <c r="B133" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C133" s="6" t="s">
+      <c r="C133" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D133" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D133" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F133" s="8"/>
     </row>
     <row r="134" s="3" customFormat="1">
       <c r="A134" s="3" t="s">
@@ -3824,19 +3852,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="136" s="4" customFormat="1">
-      <c r="A136" s="4" t="s">
+    <row r="136" s="7" customFormat="1">
+      <c r="A136" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="B136" s="6" t="s">
+      <c r="B136" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C136" s="6" t="s">
+      <c r="C136" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D136" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D136" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F136" s="8"/>
     </row>
     <row r="137" s="3" customFormat="1">
       <c r="A137" s="3" t="s">
@@ -3866,19 +3895,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="139" s="4" customFormat="1">
-      <c r="A139" s="4" t="s">
+    <row r="139" s="7" customFormat="1">
+      <c r="A139" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="B139" s="6" t="s">
+      <c r="B139" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C139" s="6" t="s">
+      <c r="C139" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D139" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D139" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F139" s="8"/>
     </row>
     <row r="140" s="3" customFormat="1">
       <c r="A140" s="3" t="s">
@@ -3908,19 +3938,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="142" s="4" customFormat="1">
-      <c r="A142" s="4" t="s">
+    <row r="142" s="7" customFormat="1">
+      <c r="A142" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="B142" s="6" t="s">
+      <c r="B142" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C142" s="6" t="s">
+      <c r="C142" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D142" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D142" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F142" s="8"/>
     </row>
     <row r="143" s="3" customFormat="1">
       <c r="A143" s="3" t="s">
@@ -3950,19 +3981,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="145" s="4" customFormat="1">
-      <c r="A145" s="4" t="s">
+    <row r="145" s="7" customFormat="1">
+      <c r="A145" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="B145" s="6" t="s">
+      <c r="B145" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C145" s="6" t="s">
+      <c r="C145" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D145" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D145" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F145" s="8"/>
     </row>
     <row r="146" s="3" customFormat="1">
       <c r="A146" s="3" t="s">
@@ -5420,19 +5452,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="250" s="4" customFormat="1">
-      <c r="A250" s="4" t="s">
+    <row r="250" s="7" customFormat="1">
+      <c r="A250" s="7" t="s">
         <v>443</v>
       </c>
-      <c r="B250" s="6" t="s">
+      <c r="B250" s="9" t="s">
         <v>444</v>
       </c>
-      <c r="C250" s="6" t="s">
+      <c r="C250" s="9" t="s">
         <v>445</v>
       </c>
-      <c r="D250" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D250" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F250" s="8"/>
     </row>
     <row r="251" s="3" customFormat="1">
       <c r="A251" s="3" t="s">
@@ -5658,19 +5691,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="267" s="4" customFormat="1">
-      <c r="A267" s="4" t="s">
+    <row r="267" s="7" customFormat="1">
+      <c r="A267" s="7" t="s">
         <v>470</v>
       </c>
-      <c r="B267" s="6" t="s">
+      <c r="B267" s="9" t="s">
         <v>444</v>
       </c>
-      <c r="C267" s="6" t="s">
+      <c r="C267" s="9" t="s">
         <v>445</v>
       </c>
-      <c r="D267" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D267" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F267" s="8"/>
     </row>
     <row r="268" s="3" customFormat="1">
       <c r="A268" s="3" t="s">
@@ -5700,19 +5734,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="270" s="4" customFormat="1">
-      <c r="A270" s="4" t="s">
+    <row r="270" s="7" customFormat="1">
+      <c r="A270" s="7" t="s">
         <v>473</v>
       </c>
-      <c r="B270" s="6" t="s">
+      <c r="B270" s="9" t="s">
         <v>474</v>
       </c>
-      <c r="C270" s="6" t="s">
+      <c r="C270" s="9" t="s">
         <v>475</v>
       </c>
-      <c r="D270" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D270" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F270" s="8"/>
     </row>
     <row r="271" s="3" customFormat="1">
       <c r="A271" s="3" t="s">
@@ -5756,19 +5791,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="274" s="4" customFormat="1">
-      <c r="A274" s="4" t="s">
+    <row r="274" s="7" customFormat="1">
+      <c r="A274" s="7" t="s">
         <v>479</v>
       </c>
-      <c r="B274" s="6" t="s">
+      <c r="B274" s="9" t="s">
         <v>480</v>
       </c>
-      <c r="C274" s="6" t="s">
+      <c r="C274" s="9" t="s">
         <v>481</v>
       </c>
-      <c r="D274" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D274" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F274" s="8"/>
     </row>
     <row r="275" s="3" customFormat="1">
       <c r="A275" s="3" t="s">
@@ -5812,19 +5848,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="278" s="4" customFormat="1">
-      <c r="A278" s="4" t="s">
+    <row r="278" s="7" customFormat="1">
+      <c r="A278" s="7" t="s">
         <v>485</v>
       </c>
-      <c r="B278" s="6" t="s">
+      <c r="B278" s="9" t="s">
         <v>486</v>
       </c>
-      <c r="C278" s="6" t="s">
+      <c r="C278" s="9" t="s">
         <v>487</v>
       </c>
-      <c r="D278" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D278" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F278" s="8"/>
     </row>
     <row r="279" s="3" customFormat="1">
       <c r="A279" s="3" t="s">
@@ -5882,19 +5919,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="283" s="4" customFormat="1">
-      <c r="A283" s="4" t="s">
+    <row r="283" s="7" customFormat="1">
+      <c r="A283" s="7" t="s">
         <v>495</v>
       </c>
-      <c r="B283" s="6" t="s">
+      <c r="B283" s="9" t="s">
         <v>474</v>
       </c>
-      <c r="C283" s="6" t="s">
+      <c r="C283" s="9" t="s">
         <v>475</v>
       </c>
-      <c r="D283" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D283" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F283" s="8"/>
     </row>
     <row r="284" s="3" customFormat="1">
       <c r="A284" s="3" t="s">
@@ -5924,19 +5962,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="286" s="4" customFormat="1">
-      <c r="A286" s="4" t="s">
+    <row r="286" s="7" customFormat="1">
+      <c r="A286" s="7" t="s">
         <v>499</v>
       </c>
-      <c r="B286" s="6" t="s">
+      <c r="B286" s="9" t="s">
         <v>480</v>
       </c>
-      <c r="C286" s="6" t="s">
+      <c r="C286" s="9" t="s">
         <v>481</v>
       </c>
-      <c r="D286" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D286" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F286" s="8"/>
     </row>
     <row r="287" s="3" customFormat="1">
       <c r="A287" s="3" t="s">
@@ -5966,28 +6005,29 @@
         <v>6</v>
       </c>
     </row>
-    <row r="289" s="4" customFormat="1">
-      <c r="A289" s="4" t="s">
+    <row r="289" s="7" customFormat="1">
+      <c r="A289" s="7" t="s">
         <v>503</v>
       </c>
-      <c r="B289" s="6" t="s">
+      <c r="B289" s="9" t="s">
         <v>486</v>
       </c>
-      <c r="C289" s="6" t="s">
+      <c r="C289" s="9" t="s">
         <v>487</v>
       </c>
-      <c r="D289" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D289" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F289" s="8"/>
     </row>
     <row r="290" s="3" customFormat="1">
       <c r="A290" s="3" t="s">
         <v>504</v>
       </c>
-      <c r="B290" s="5" t="s">
+      <c r="B290" s="10" t="s">
         <v>505</v>
       </c>
-      <c r="C290" s="6" t="s">
+      <c r="C290" s="9" t="s">
         <v>506</v>
       </c>
       <c r="D290" s="3" t="s">

</xml_diff>